<commit_message>
adjustments to code, based on 1. review round; exclusion of south africa and netherlands; inclusion of omega; switch to one-sided testing
</commit_message>
<xml_diff>
--- a/means_t-results.xlsx
+++ b/means_t-results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c63a7df432fff15/Desktop/workshops/GitHub_23/mev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_0F057FD68F79A8D366075C52F37BD2724ACB7AE5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EF81EB6-6B55-45B6-BABC-5DC2DBE2AFD6}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_CC6AFDCE8F79A8D366075C52F31082F001A4ADFE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFF1436D-AE82-4D6D-88E7-EBDC9D61321A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>rowname</t>
   </si>
@@ -31,7 +31,7 @@
     <t>core_good_lo</t>
   </si>
   <si>
-    <t>3.95 (0.82)</t>
+    <t>3.91 (0.75)</t>
   </si>
   <si>
     <t>3.94 (0.72)</t>
@@ -40,16 +40,10 @@
     <t>3.87 (0.78)</t>
   </si>
   <si>
-    <t>3.9 (0.85)</t>
-  </si>
-  <si>
-    <t>4.1 (0.88)</t>
-  </si>
-  <si>
     <t>core_good_he</t>
   </si>
   <si>
-    <t>3.99 (0.75)</t>
+    <t>4 (0.78)</t>
   </si>
   <si>
     <t>3.9 (0.76)</t>
@@ -58,34 +52,22 @@
     <t>4.08 (0.78)</t>
   </si>
   <si>
-    <t>4 (0.7)</t>
+    <t>value_comm_lo</t>
   </si>
   <si>
     <t>3.98 (0.76)</t>
   </si>
   <si>
-    <t>value_comm_lo</t>
-  </si>
-  <si>
-    <t>4 (0.77)</t>
-  </si>
-  <si>
     <t>4 (0.8)</t>
   </si>
   <si>
     <t>3.96 (0.73)</t>
   </si>
   <si>
-    <t>3.96 (0.8)</t>
-  </si>
-  <si>
-    <t>4.06 (0.77)</t>
-  </si>
-  <si>
     <t>value_comm_he</t>
   </si>
   <si>
-    <t>3.97 (0.74)</t>
+    <t>4 (0.71)</t>
   </si>
   <si>
     <t>3.85 (0.69)</t>
@@ -94,16 +76,10 @@
     <t>4.13 (0.71)</t>
   </si>
   <si>
-    <t>4.03 (0.77)</t>
-  </si>
-  <si>
-    <t>3.84 (0.75)</t>
-  </si>
-  <si>
     <t>pay_deservingness_lo</t>
   </si>
   <si>
-    <t>24.13 (21.17)</t>
+    <t>35.33 (25.76)</t>
   </si>
   <si>
     <t>12.02 (3.68)</t>
@@ -112,16 +88,10 @@
     <t>56.43 (17.67)</t>
   </si>
   <si>
-    <t>14.91 (4.27)</t>
-  </si>
-  <si>
-    <t>12.3 (3.47)</t>
-  </si>
-  <si>
     <t>pay_deservingness_he</t>
   </si>
   <si>
-    <t>24.35 (21.85)</t>
+    <t>36.28 (26.32)</t>
   </si>
   <si>
     <t>11.95 (3.53)</t>
@@ -130,16 +100,10 @@
     <t>58.29 (16.87)</t>
   </si>
   <si>
-    <t>14.3 (3.94)</t>
-  </si>
-  <si>
-    <t>11.98 (3.61)</t>
-  </si>
-  <si>
     <t>warmth_lo</t>
   </si>
   <si>
-    <t>3.98 (2.01)</t>
+    <t>4.11 (2.03)</t>
   </si>
   <si>
     <t>4.04 (2.06)</t>
@@ -148,16 +112,10 @@
     <t>4.17 (2)</t>
   </si>
   <si>
-    <t>3.79 (2.01)</t>
-  </si>
-  <si>
-    <t>3.91 (1.97)</t>
-  </si>
-  <si>
     <t>warmth_he</t>
   </si>
   <si>
-    <t>4.04 (1.98)</t>
+    <t>4.12 (1.98)</t>
   </si>
   <si>
     <t>4.13 (1.94)</t>
@@ -166,16 +124,10 @@
     <t>4.1 (2.02)</t>
   </si>
   <si>
-    <t>4.04 (1.94)</t>
-  </si>
-  <si>
-    <t>3.88 (2.03)</t>
-  </si>
-  <si>
     <t>competence_lo</t>
   </si>
   <si>
-    <t>3.98 (2.02)</t>
+    <t>3.97 (2.03)</t>
   </si>
   <si>
     <t>3.93 (2.06)</t>
@@ -184,28 +136,16 @@
     <t>4 (2.01)</t>
   </si>
   <si>
-    <t>4.25 (1.93)</t>
-  </si>
-  <si>
-    <t>3.73 (2.06)</t>
-  </si>
-  <si>
     <t>competence_he</t>
   </si>
   <si>
-    <t>3.94 (2.03)</t>
+    <t>4.07 (1.99)</t>
   </si>
   <si>
     <t>3.94 (1.99)</t>
   </si>
   <si>
     <t>4.19 (1.99)</t>
-  </si>
-  <si>
-    <t>3.84 (2.13)</t>
-  </si>
-  <si>
-    <t>3.8 (2.01)</t>
   </si>
 </sst>
 </file>
@@ -558,16 +498,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -604,23 +543,23 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -628,34 +567,34 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -663,7 +602,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -671,71 +610,71 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -743,239 +682,79 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>56</v>
-      </c>
-      <c r="B47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>56</v>
-      </c>
-      <c r="B49" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>56</v>
-      </c>
-      <c r="B51" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>